<commit_message>
Update Excel sample file.
</commit_message>
<xml_diff>
--- a/tests/sample-files/simple-list.xlsx
+++ b/tests/sample-files/simple-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodolfo/Projects/LACCEI/Digital-Certificates/tests/sample-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{959F1471-87F9-A84C-8FF9-6FFCDE7E6A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39767F02-015A-C542-9398-57F08D28931D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2120" windowWidth="28040" windowHeight="17440" xr2:uid="{044CAF24-F9AE-F14C-9126-8E93B4C8D4D3}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Chemistry</t>
+  </si>
+  <si>
+    <t>10/1/2023</t>
+  </si>
+  <si>
+    <t>10/2/2023</t>
+  </si>
+  <si>
+    <t>10/3/2023</t>
   </si>
 </sst>
 </file>
@@ -532,7 +541,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -910,7 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E956935-E2E2-364B-ADCD-293C27080612}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -929,8 +940,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>45200</v>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -940,8 +951,8 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>45201</v>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -951,8 +962,8 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>45202</v>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>

</xml_diff>